<commit_message>
add d17O to scale decompression
</commit_message>
<xml_diff>
--- a/m-isotopomer/00_MATLAB_template.xlsx
+++ b/m-isotopomer/00_MATLAB_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/Spec Calibration Files/Scrambling R&amp;D/pyScramble/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/Spec Calibration Files/N2O_isotopocule_data_corrections/m-isotopomer/m-isotopomer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB363D7-76B4-B64D-BDAE-0C8A26048A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11DA931-0BB0-4E4A-97D5-B04963CD2CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18140" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -1359,6 +1359,121 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6410-E54E-9C39-579B1B44A44F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>d17O</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scale_decompression!$F$9:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23.653181412339649</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.218968675425501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.517499686386948</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scale_decompression!$F$4:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>22.618966808462872</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.430518925956932</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.757033254469313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8074-A446-9AC9-FF7513B94E3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2558,8 +2673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="AY22" sqref="AY22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2878,7 +2993,7 @@
         <v>2.1171008279007989E-3</v>
       </c>
       <c r="AK3" s="73">
-        <f>A3</f>
+        <f t="shared" ref="AK3:AK17" si="1">A3</f>
         <v>201204</v>
       </c>
       <c r="AL3" t="str">
@@ -2924,8 +3039,8 @@
         <v>5.8493223399717582</v>
       </c>
       <c r="AY3" s="78">
-        <f>AQ3</f>
-        <v>24.2603773951218</v>
+        <f>AQ3*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>23.28974545578863</v>
       </c>
       <c r="AZ3" s="78">
         <f>AR3*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -2993,7 +3108,7 @@
         <v>0.42930239999999997</v>
       </c>
       <c r="Z4" s="46">
-        <f t="shared" ref="Z4:AB32" si="1">N4/R4</f>
+        <f t="shared" ref="Z4:AB32" si="2">N4/R4</f>
         <v>0.99630401210059016</v>
       </c>
       <c r="AA4" s="47">
@@ -3005,36 +3120,36 @@
         <v>1.0004234777164069</v>
       </c>
       <c r="AD4" s="49">
-        <f t="shared" ref="AD4:AD24" si="2">$V$7*(20-H4)+AB4</f>
+        <f t="shared" ref="AD4:AD24" si="3">$V$7*(20-H4)+AB4</f>
         <v>1.0011999046840065</v>
       </c>
       <c r="AE4" s="49">
-        <f t="shared" ref="AE4:AE24" si="3">$W$7*(20-H4)+Z4</f>
+        <f t="shared" ref="AE4:AE24" si="4">$W$7*(20-H4)+Z4</f>
         <v>0.99668972770557829</v>
       </c>
       <c r="AF4" s="49">
-        <f t="shared" ref="AF4:AF24" si="4">$X$7*(20-H4)+AA4</f>
+        <f t="shared" ref="AF4:AF24" si="5">$X$7*(20-H4)+AA4</f>
         <v>0.99497700286985102</v>
       </c>
       <c r="AG4" s="50"/>
       <c r="AH4" s="51">
-        <f t="shared" ref="AH4:AH24" si="5">AD4*$V$3</f>
+        <f t="shared" ref="AH4:AH24" si="6">AD4*$V$3</f>
         <v>3.7382429851740414E-3</v>
       </c>
       <c r="AI4" s="51">
-        <f t="shared" ref="AI4:AI16" si="6">AE4*$W$3</f>
+        <f t="shared" ref="AI4:AI16" si="7">AE4*$W$3</f>
         <v>7.7154000492014665E-3</v>
       </c>
       <c r="AJ4" s="51">
-        <f t="shared" ref="AJ4:AJ24" si="7">AF4*$X$3</f>
+        <f t="shared" ref="AJ4:AJ24" si="8">AF4*$X$3</f>
         <v>2.0907404217080498E-3</v>
       </c>
       <c r="AK4" s="73">
-        <f>A4</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL4" s="66" t="str">
-        <f t="shared" ref="AL4:AL17" si="8">C4</f>
+        <f t="shared" ref="AL4:AL17" si="9">C4</f>
         <v>S2_ref_1</v>
       </c>
       <c r="AM4" s="82">
@@ -3068,16 +3183,16 @@
         <v>-12.372403732904573</v>
       </c>
       <c r="AW4" s="78">
-        <f t="shared" ref="AW4:AW17" si="9">AU4-AV4</f>
+        <f t="shared" ref="AW4:AW17" si="10">AU4-AV4</f>
         <v>18.688527112829505</v>
       </c>
       <c r="AX4" s="78">
-        <f t="shared" ref="AX4:AX17" si="10">AVERAGE(AU4:AV4)</f>
+        <f t="shared" ref="AX4:AX17" si="11">AVERAGE(AU4:AV4)</f>
         <v>-3.0281401764898201</v>
       </c>
       <c r="AY4" s="78">
-        <f t="shared" ref="AY4:AY17" si="11">AQ4</f>
-        <v>17.6812819742809</v>
+        <f>AQ4*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>16.940962612526206</v>
       </c>
       <c r="AZ4" s="78">
         <f>AR4*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -3150,7 +3265,7 @@
       <c r="W5" s="14"/>
       <c r="X5" s="15"/>
       <c r="Z5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0004165843625989</v>
       </c>
       <c r="AA5" s="47">
@@ -3162,36 +3277,36 @@
         <v>0.99713138761787079</v>
       </c>
       <c r="AD5" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99706434207705574</v>
       </c>
       <c r="AE5" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0003832772874761</v>
       </c>
       <c r="AF5" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0043106480077921</v>
       </c>
       <c r="AG5" s="50"/>
       <c r="AH5" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7228017752489757E-3</v>
       </c>
       <c r="AI5" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.743991908667606E-3</v>
       </c>
       <c r="AJ5" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1103531656362878E-3</v>
       </c>
       <c r="AK5" s="73">
-        <f>A5</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL5" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>B6_ref_1</v>
       </c>
       <c r="AM5" s="82">
@@ -3223,16 +3338,16 @@
         <v>1.0580306501241861</v>
       </c>
       <c r="AW5" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1.8873324132551577</v>
       </c>
       <c r="AX5" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.11436444349660724</v>
       </c>
       <c r="AY5" s="78">
-        <f t="shared" si="11"/>
-        <v>22.603672551350499</v>
+        <f>AQ5*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>21.691036421235573</v>
       </c>
       <c r="AZ5" s="78">
         <f>AR5*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -3309,7 +3424,7 @@
         <v>36</v>
       </c>
       <c r="Z6" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0059841490064783</v>
       </c>
       <c r="AA6" s="47">
@@ -3321,36 +3436,36 @@
         <v>1.008564673064511</v>
       </c>
       <c r="AD6" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0094138034244713</v>
       </c>
       <c r="AE6" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0064059824102283</v>
       </c>
       <c r="AF6" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0077071570383731</v>
       </c>
       <c r="AG6" s="50"/>
       <c r="AH6" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7689117349450109E-3</v>
       </c>
       <c r="AI6" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7906138192870506E-3</v>
       </c>
       <c r="AJ6" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1174902338322861E-3</v>
       </c>
       <c r="AK6" s="73">
-        <f>A6</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="AM6" s="78">
@@ -3382,16 +3497,16 @@
         <v>-1.4461946306102322</v>
       </c>
       <c r="AW6" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.989776332854744</v>
       </c>
       <c r="AX6" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.5486935358171392</v>
       </c>
       <c r="AY6" s="78">
-        <f t="shared" si="11"/>
-        <v>24.352429878149199</v>
+        <f>AQ6*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>23.378575482949014</v>
       </c>
       <c r="AZ6" s="78">
         <f>AR6*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -3468,7 +3583,7 @@
         <v>4.8711468260038703E-5</v>
       </c>
       <c r="Z7" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99710210962534773</v>
       </c>
       <c r="AA7" s="47">
@@ -3480,36 +3595,36 @@
         <v>1.0019882509476716</v>
       </c>
       <c r="AD7" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0010419752766739</v>
       </c>
       <c r="AE7" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99663201609671503</v>
       </c>
       <c r="AF7" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.9951628615034982</v>
       </c>
       <c r="AG7" s="50"/>
       <c r="AH7" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7376533142238627E-3</v>
       </c>
       <c r="AI7" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7149533021973731E-3</v>
       </c>
       <c r="AJ7" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.091130965566821E-3</v>
       </c>
       <c r="AK7" s="73">
-        <f>A7</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>S2_ref_2</v>
       </c>
       <c r="AM7" s="78">
@@ -3541,16 +3656,16 @@
         <v>-12.29547383021416</v>
       </c>
       <c r="AW7" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>18.394866213540318</v>
       </c>
       <c r="AX7" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-3.0980407234440004</v>
       </c>
       <c r="AY7" s="78">
-        <f t="shared" si="11"/>
-        <v>17.7806714278295</v>
+        <f>AQ7*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>17.036872766905748</v>
       </c>
       <c r="AZ7" s="78">
         <f>AR7*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -3618,7 +3733,7 @@
         <v>0.42855359999999998</v>
       </c>
       <c r="Z8" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99919974572438763</v>
       </c>
       <c r="AA8" s="47">
@@ -3630,36 +3745,36 @@
         <v>0.99635331496456925</v>
       </c>
       <c r="AD8" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99629481277958798</v>
       </c>
       <c r="AE8" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99917068284195976</v>
       </c>
       <c r="AF8" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0023860907979212</v>
       </c>
       <c r="AG8" s="50"/>
       <c r="AH8" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7199285353648262E-3</v>
       </c>
       <c r="AI8" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7346051848110903E-3</v>
       </c>
       <c r="AJ8" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1063091027675373E-3</v>
       </c>
       <c r="AK8" s="73">
-        <f>A8</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>B6_ref_2</v>
       </c>
       <c r="AM8" s="83">
@@ -3691,16 +3806,16 @@
         <v>-0.63444166305131089</v>
       </c>
       <c r="AW8" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.84785348286075435</v>
       </c>
       <c r="AX8" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.0583684044816881</v>
       </c>
       <c r="AY8" s="78">
-        <f t="shared" si="11"/>
-        <v>21.5940737361231</v>
+        <f>AQ8*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>20.716780353085323</v>
       </c>
       <c r="AZ8" s="78">
         <f>AR8*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -3768,7 +3883,7 @@
         <v>0.42850050000000001</v>
       </c>
       <c r="Z9" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0046720367967517</v>
       </c>
       <c r="AA9" s="47">
@@ -3780,35 +3895,35 @@
         <v>1.0090592659751856</v>
       </c>
       <c r="AD9" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0099089621203003</v>
       </c>
       <c r="AE9" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0050941512728657</v>
       </c>
       <c r="AF9" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0057116133646442</v>
       </c>
       <c r="AH9" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.770760540076305E-3</v>
       </c>
       <c r="AI9" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7804589017230353E-3</v>
       </c>
       <c r="AJ9" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1132970074462343E-3</v>
       </c>
       <c r="AK9" s="73">
-        <f>A9</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL9" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ATM_EQ_SW_2</v>
       </c>
       <c r="AM9" s="82">
@@ -3839,16 +3954,16 @@
         <v>-4.9634141411132422</v>
       </c>
       <c r="AW9" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.617501578245424</v>
       </c>
       <c r="AX9" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.3453366480094697</v>
       </c>
       <c r="AY9" s="78">
-        <f t="shared" si="11"/>
-        <v>23.3079288441653</v>
+        <f>AQ9*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>22.370639008381321</v>
       </c>
       <c r="AZ9" s="78">
         <f>AR9*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -3914,7 +4029,7 @@
         <v>0.42850440000000001</v>
       </c>
       <c r="Z10" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99084318862083898</v>
       </c>
       <c r="AA10" s="47">
@@ -3926,35 +4041,35 @@
         <v>1.0057661018183244</v>
       </c>
       <c r="AD10" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0059352715795371</v>
       </c>
       <c r="AE10" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99092722925764687</v>
       </c>
       <c r="AF10" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0049378092932522</v>
       </c>
       <c r="AH10" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7559237220544848E-3</v>
       </c>
       <c r="AI10" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.6707924049438676E-3</v>
       </c>
       <c r="AJ10" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1116710166485821E-3</v>
       </c>
       <c r="AK10" s="73">
-        <f>A10</f>
+        <f t="shared" si="1"/>
         <v>201205</v>
       </c>
       <c r="AL10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DI</v>
       </c>
       <c r="AM10" s="78">
@@ -3985,16 +4100,16 @@
         <v>-30.856862325423542</v>
       </c>
       <c r="AW10" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.290905052980889</v>
       </c>
       <c r="AX10" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-8.7114097989330954</v>
       </c>
       <c r="AY10" s="78">
-        <f t="shared" si="11"/>
-        <v>23.011923180081201</v>
+        <f>AQ10*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>22.084995532882765</v>
       </c>
       <c r="AZ10" s="78">
         <f>AR10*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4060,7 +4175,7 @@
         <v>0.42918780000000001</v>
       </c>
       <c r="Z11" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0052879196564961</v>
       </c>
       <c r="AA11" s="47">
@@ -4072,35 +4187,35 @@
         <v>1.0099504226354989</v>
       </c>
       <c r="AD11" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0108187331121987</v>
       </c>
       <c r="AE11" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0057192814133826</v>
       </c>
       <c r="AF11" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0054625917600983</v>
       </c>
       <c r="AH11" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7741574091857285E-3</v>
       </c>
       <c r="AI11" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7852980497375374E-3</v>
       </c>
       <c r="AJ11" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1127737395385329E-3</v>
       </c>
       <c r="AK11" s="73">
-        <f>A11</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL11" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="AM11" s="82">
@@ -4131,16 +4246,16 @@
         <v>-4.7573166711320791</v>
       </c>
       <c r="AW11" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21.536799035371125</v>
       </c>
       <c r="AX11" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.0110828465534825</v>
       </c>
       <c r="AY11" s="78">
-        <f t="shared" si="11"/>
-        <v>23.171307203657499</v>
+        <f>AQ11*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>22.238800043935441</v>
       </c>
       <c r="AZ11" s="78">
         <f>AR11*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4206,7 +4321,7 @@
         <v>0.42925489999999999</v>
       </c>
       <c r="Z12" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99606571006022826</v>
       </c>
       <c r="AA12" s="47">
@@ -4218,35 +4333,35 @@
         <v>1.0004901516558111</v>
       </c>
       <c r="AD12" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0011869726521643</v>
       </c>
       <c r="AE12" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99641187878361481</v>
       </c>
       <c r="AF12" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.99378130442821833</v>
       </c>
       <c r="AH12" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7381947000342886E-3</v>
       </c>
       <c r="AI12" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7132492137643215E-3</v>
       </c>
       <c r="AJ12" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.0882279062862017E-3</v>
       </c>
       <c r="AK12" s="73">
-        <f>A12</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL12" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>S2_ref_1</v>
       </c>
       <c r="AM12" s="82">
@@ -4277,16 +4392,16 @@
         <v>-12.976889665931125</v>
       </c>
       <c r="AW12" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>19.419594918399067</v>
       </c>
       <c r="AX12" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-3.2670922067315917</v>
       </c>
       <c r="AY12" s="78">
-        <f t="shared" si="11"/>
-        <v>17.047650523571001</v>
+        <f>AQ12*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>16.329512523130131</v>
       </c>
       <c r="AZ12" s="78">
         <f>AR12*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4352,7 +4467,7 @@
         <v>0.4290465</v>
       </c>
       <c r="Z13" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0001949751810382</v>
       </c>
       <c r="AA13" s="47">
@@ -4364,35 +4479,35 @@
         <v>0.9974865195264383</v>
       </c>
       <c r="AD13" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99745574081403032</v>
       </c>
       <c r="AE13" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0001796848444418</v>
       </c>
       <c r="AF13" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0040343543858852</v>
       </c>
       <c r="AH13" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7242631653031056E-3</v>
       </c>
       <c r="AI13" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7424158944865221E-3</v>
       </c>
       <c r="AJ13" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1097725911688229E-3</v>
       </c>
       <c r="AK13" s="73">
-        <f>A13</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL13" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>B6_ref_1</v>
       </c>
       <c r="AM13" s="82">
@@ -4423,16 +4538,16 @@
         <v>0.11297104454439499</v>
       </c>
       <c r="AW13" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-0.34045204002409357</v>
       </c>
       <c r="AX13" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-5.7254975467651792E-2</v>
       </c>
       <c r="AY13" s="78">
-        <f t="shared" si="11"/>
-        <v>22.459159738802899</v>
+        <f>AQ13*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>21.551582528831542</v>
       </c>
       <c r="AZ13" s="78">
         <f>AR13*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4498,7 +4613,7 @@
         <v>0.42774570000000001</v>
       </c>
       <c r="Z14" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0044547573920082</v>
       </c>
       <c r="AA14" s="47">
@@ -4510,35 +4625,35 @@
         <v>1.0078193655716468</v>
       </c>
       <c r="AD14" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0086764735022862</v>
       </c>
       <c r="AE14" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0048805539160894</v>
       </c>
       <c r="AF14" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0053599727245706</v>
       </c>
       <c r="AH14" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7661587198913019E-3</v>
       </c>
       <c r="AI14" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7788054392550566E-3</v>
       </c>
       <c r="AJ14" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1125581066495356E-3</v>
       </c>
       <c r="AK14" s="73">
-        <f>A14</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL14" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ATM_EQ_SW_2</v>
       </c>
       <c r="AM14" s="84">
@@ -4568,16 +4683,16 @@
         <v>-3.8676302133328111</v>
       </c>
       <c r="AW14" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17.901214612788912</v>
       </c>
       <c r="AX14" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.082977093061646</v>
       </c>
       <c r="AY14" s="78">
-        <f t="shared" si="11"/>
-        <v>23.1234883652725</v>
+        <f>AQ14*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>22.192655186427871</v>
       </c>
       <c r="AZ14" s="78">
         <f>AR14*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4643,7 +4758,7 @@
         <v>0.42802899999999999</v>
       </c>
       <c r="Z15" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0052059357909202</v>
       </c>
       <c r="AA15" s="47">
@@ -4655,35 +4770,35 @@
         <v>1.009640935544087</v>
       </c>
       <c r="AD15" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0105121315250749</v>
       </c>
       <c r="AE15" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0056387310168626</v>
       </c>
       <c r="AF15" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0064676550191509</v>
       </c>
       <c r="AH15" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7730126315774341E-3</v>
       </c>
       <c r="AI15" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7846745071083745E-3</v>
       </c>
       <c r="AJ15" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1148856741621614E-3</v>
       </c>
       <c r="AK15" s="73">
-        <f>A15</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ATM_EQ_SW_3</v>
       </c>
       <c r="AM15" s="83">
@@ -4713,16 +4828,16 @@
         <v>-4.5318745625365429</v>
       </c>
       <c r="AW15" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.840331805270921</v>
       </c>
       <c r="AX15" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.8882913400989167</v>
       </c>
       <c r="AY15" s="78">
-        <f t="shared" si="11"/>
-        <v>23.703556787671602</v>
+        <f>AQ15*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>22.752417313661923</v>
       </c>
       <c r="AZ15" s="78">
         <f>AR15*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4788,7 +4903,7 @@
         <v>0.42812329999999998</v>
       </c>
       <c r="Z16" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99600394236024603</v>
       </c>
       <c r="AA16" s="47">
@@ -4800,35 +4915,35 @@
         <v>1.0006194477151793</v>
       </c>
       <c r="AD16" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0012823781807745</v>
       </c>
       <c r="AE16" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99633327484903467</v>
       </c>
       <c r="AF16" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.99474403428411884</v>
       </c>
       <c r="AH16" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7385509216503769E-3</v>
       </c>
       <c r="AI16" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.7126407387455983E-3</v>
       </c>
       <c r="AJ16" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.0902508859320735E-3</v>
       </c>
       <c r="AK16" s="73">
-        <f>A16</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL16" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>S2_ref_2</v>
       </c>
       <c r="AM16" s="83">
@@ -4858,16 +4973,16 @@
         <v>-13.258229096818942</v>
       </c>
       <c r="AW16" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>19.783632296490552</v>
       </c>
       <c r="AX16" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-3.3664129485736662</v>
       </c>
       <c r="AY16" s="78">
-        <f t="shared" si="11"/>
-        <v>17.560394819866399</v>
+        <f>AQ16*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>16.824307321361651</v>
       </c>
       <c r="AZ16" s="78">
         <f>AR16*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -4933,7 +5048,7 @@
         <v>0.42825439999999998</v>
       </c>
       <c r="Z17" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99331504606302035</v>
       </c>
       <c r="AA17" s="47">
@@ -4945,19 +5060,19 @@
         <v>1.0055340937536195</v>
       </c>
       <c r="AD17" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0058961962525363</v>
       </c>
       <c r="AE17" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99349493237592013</v>
       </c>
       <c r="AF17" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0044001925480899</v>
       </c>
       <c r="AH17" s="51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7557778240511282E-3</v>
       </c>
       <c r="AI17" s="51">
@@ -4965,15 +5080,15 @@
         <v>7.6906690588456452E-3</v>
       </c>
       <c r="AJ17" s="51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1105413251509336E-3</v>
       </c>
       <c r="AK17" s="73">
-        <f>A17</f>
+        <f t="shared" si="1"/>
         <v>201207</v>
       </c>
       <c r="AL17" s="66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DI</v>
       </c>
       <c r="AM17" s="84">
@@ -5003,16 +5118,16 @@
         <v>-25.206531833767624</v>
       </c>
       <c r="AW17" s="78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>38.046365461704063</v>
       </c>
       <c r="AX17" s="78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-6.1833491029155914</v>
       </c>
       <c r="AY17" s="78">
-        <f t="shared" si="11"/>
-        <v>22.706668195684699</v>
+        <f>AQ17*scale_decompression!F$14+scale_decompression!F$15</f>
+        <v>21.790426525475187</v>
       </c>
       <c r="AZ17" s="78">
         <f>AR17*scale_decompression!G$14+scale_decompression!G$15</f>
@@ -5039,7 +5154,7 @@
       <c r="S18" s="42"/>
       <c r="T18" s="42"/>
       <c r="Z18" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA18" s="47" t="e">
@@ -5051,19 +5166,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AD18" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE18" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF18" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH18" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI18" s="51" t="e">
@@ -5071,7 +5186,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ18" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK18" s="76"/>
@@ -5104,31 +5219,31 @@
       <c r="S19" s="42"/>
       <c r="T19" s="42"/>
       <c r="Z19" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA19" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB19" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD19" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE19" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF19" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH19" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI19" s="51" t="e">
@@ -5136,7 +5251,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ19" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK19" s="76"/>
@@ -5169,31 +5284,31 @@
       <c r="S20" s="42"/>
       <c r="T20" s="42"/>
       <c r="Z20" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA20" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB20" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD20" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE20" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF20" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH20" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI20" s="51" t="e">
@@ -5201,7 +5316,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ20" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK20" s="76"/>
@@ -5234,31 +5349,31 @@
       <c r="S21" s="42"/>
       <c r="T21" s="42"/>
       <c r="Z21" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA21" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB21" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD21" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE21" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF21" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH21" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI21" s="51" t="e">
@@ -5266,7 +5381,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ21" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK21" s="76"/>
@@ -5299,31 +5414,31 @@
       <c r="S22" s="42"/>
       <c r="T22" s="42"/>
       <c r="Z22" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA22" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB22" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD22" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE22" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF22" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH22" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI22" s="51" t="e">
@@ -5331,7 +5446,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ22" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK22" s="76"/>
@@ -5364,31 +5479,31 @@
       <c r="S23" s="42"/>
       <c r="T23" s="42"/>
       <c r="Z23" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA23" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB23" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD23" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE23" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF23" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH23" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI23" s="51" t="e">
@@ -5396,7 +5511,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ23" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK23" s="76"/>
@@ -5429,31 +5544,31 @@
       <c r="S24" s="42"/>
       <c r="T24" s="42"/>
       <c r="Z24" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA24" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB24" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD24" s="49" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE24" s="49" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF24" s="49" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH24" s="51" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI24" s="51" t="e">
@@ -5461,7 +5576,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AJ24" s="51" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK24" s="76"/>
@@ -5494,15 +5609,15 @@
       <c r="S25" s="42"/>
       <c r="T25" s="42"/>
       <c r="Z25" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA25" s="47" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB25" s="48" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD25" s="49" t="e">
@@ -5559,7 +5674,7 @@
       <c r="S26" s="42"/>
       <c r="T26" s="42"/>
       <c r="Z26" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA26" s="47" t="e">
@@ -5624,7 +5739,7 @@
       <c r="S27" s="42"/>
       <c r="T27" s="42"/>
       <c r="Z27" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA27" s="47" t="e">
@@ -5689,7 +5804,7 @@
       <c r="S28" s="42"/>
       <c r="T28" s="42"/>
       <c r="Z28" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA28" s="47" t="e">
@@ -5754,7 +5869,7 @@
       <c r="S29" s="42"/>
       <c r="T29" s="42"/>
       <c r="Z29" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA29" s="47" t="e">
@@ -5819,7 +5934,7 @@
       <c r="S30" s="42"/>
       <c r="T30" s="42"/>
       <c r="Z30" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA30" s="47" t="e">
@@ -5884,7 +5999,7 @@
       <c r="S31" s="42"/>
       <c r="T31" s="42"/>
       <c r="Z31" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA31" s="47" t="e">
@@ -5949,7 +6064,7 @@
       <c r="S32" s="42"/>
       <c r="T32" s="42"/>
       <c r="Z32" s="46" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA32" s="47" t="e">
@@ -7718,8 +7833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7789,7 +7904,10 @@
         <f>AVERAGE(B4:C4)</f>
         <v>6.1999999999999993</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="57">
+        <f>((G4/1000+1)^0.516-1)*1000</f>
+        <v>22.618966808462872</v>
+      </c>
       <c r="G4" s="57">
         <v>44.3</v>
       </c>
@@ -7810,7 +7928,10 @@
       <c r="E5" s="57">
         <v>-0.27605719255555561</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="57">
+        <f t="shared" ref="F5:F6" si="0">((G5/1000+1)^0.516-1)*1000</f>
+        <v>21.430518925956932</v>
+      </c>
       <c r="G5" s="57">
         <v>41.949257311111111</v>
       </c>
@@ -7831,7 +7952,10 @@
       <c r="E6" s="57">
         <v>-3.66</v>
       </c>
-      <c r="F6" s="57"/>
+      <c r="F6" s="57">
+        <f t="shared" si="0"/>
+        <v>16.757033254469313</v>
+      </c>
       <c r="G6" s="57">
         <v>32.729999999999997</v>
       </c>
@@ -7975,9 +8099,12 @@
       </c>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="F14" s="59">
+        <f>SLOPE(F4:F6,F9:F11)</f>
+        <v>0.96499327599826168</v>
+      </c>
       <c r="G14" s="59">
-        <f t="shared" ref="G14" si="0">SLOPE(G4:G6,G9:G11)</f>
+        <f t="shared" ref="G14" si="1">SLOPE(G4:G6,G9:G11)</f>
         <v>0.96419175756222808</v>
       </c>
     </row>
@@ -7995,9 +8122,12 @@
       </c>
       <c r="D15" s="57"/>
       <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
+      <c r="F15" s="57">
+        <f>INTERCEPT(F4:F6,F9:F11)</f>
+        <v>-0.12135560368412968</v>
+      </c>
       <c r="G15" s="57">
-        <f t="shared" ref="G15" si="1">INTERCEPT(G4:G6,G9:G11)</f>
+        <f t="shared" ref="G15" si="2">INTERCEPT(G4:G6,G9:G11)</f>
         <v>-0.22057002510575074</v>
       </c>
     </row>
@@ -8015,11 +8145,11 @@
         <v>56</v>
       </c>
       <c r="B17" s="57">
-        <f t="shared" ref="B17:C19" si="2">B$15+B$14*B9</f>
+        <f t="shared" ref="B17:C19" si="3">B$15+B$14*B9</f>
         <v>15.346487892548804</v>
       </c>
       <c r="C17" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.771253291378001</v>
       </c>
       <c r="D17" s="57">
@@ -8030,7 +8160,10 @@
         <f>AVERAGE(B17:C17)</f>
         <v>5.7876173005854019</v>
       </c>
-      <c r="F17" s="57"/>
+      <c r="F17" s="57">
+        <f>F$15+F$14*F9</f>
+        <v>22.703805415190697</v>
+      </c>
       <c r="G17" s="57">
         <f>G$15+G$14*G9</f>
         <v>44.467772503530497</v>
@@ -8041,11 +8174,11 @@
         <v>57</v>
       </c>
       <c r="B18" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.84635930150757854</v>
       </c>
       <c r="C18" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17885334387242335</v>
       </c>
       <c r="D18" s="57">
@@ -8053,10 +8186,13 @@
         <v>-1.0252126453800019</v>
       </c>
       <c r="E18" s="57">
-        <f t="shared" ref="E18:E19" si="3">AVERAGE(B18:C18)</f>
+        <f t="shared" ref="E18:E19" si="4">AVERAGE(B18:C18)</f>
         <v>-0.33375297881757759</v>
       </c>
-      <c r="F18" s="57"/>
+      <c r="F18" s="57">
+        <f t="shared" ref="F18:F19" si="5">F$15+F$14*F10</f>
+        <v>21.31979976771748</v>
+      </c>
       <c r="G18" s="57">
         <f>G$15+G$14*G10</f>
         <v>41.730160131465027</v>
@@ -8067,11 +8203,11 @@
         <v>58</v>
       </c>
       <c r="B19" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3459060538476608</v>
       </c>
       <c r="C19" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-12.725749081467198</v>
       </c>
       <c r="D19" s="57">
@@ -8079,10 +8215,13 @@
         <v>19.07165513531486</v>
       </c>
       <c r="E19" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.1899215138097685</v>
       </c>
-      <c r="F19" s="57"/>
+      <c r="F19" s="57">
+        <f t="shared" si="5"/>
+        <v>16.782913805980932</v>
+      </c>
       <c r="G19" s="57">
         <f>G$15+G$14*G11</f>
         <v>32.781324676115581</v>

</xml_diff>

<commit_message>
Reference delta vals. directly to AIR
</commit_message>
<xml_diff>
--- a/m-isotopomer/00_MATLAB_template.xlsx
+++ b/m-isotopomer/00_MATLAB_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colette/Box Sync/N2O Research/Spec Calibration Files/N2O_isotopocule_data_corrections/m-isotopomer/m-isotopomer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11DA931-0BB0-4E4A-97D5-B04963CD2CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB069922-DBF8-2644-AD5F-14A98E6DDF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18140" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -807,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -973,6 +973,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,13 +1098,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14.416870498714482</c:v>
+                  <c:v>15.0861773640476</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.5626976748263186</c:v>
+                  <c:v>-0.89602718804360248</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5348370076648328</c:v>
+                  <c:v>6.1979586386672905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1211,13 +1213,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-2.9218372565587871</c:v>
+                  <c:v>-3.5911483585576711</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2897969450214886</c:v>
+                  <c:v>0.6231269711594033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-12.469189824435823</c:v>
+                  <c:v>-13.132315831232798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1326,13 +1328,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46.347982315905767</c:v>
+                  <c:v>46.348063533077784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.508700243025373</c:v>
+                  <c:v>43.508690422415036</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.227522111016825</c:v>
+                  <c:v>34.22760552609693</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1441,13 +1443,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23.653181412339649</c:v>
+                  <c:v>23.653222412870818</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.218968675425501</c:v>
+                  <c:v>22.218963711612133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.517499686386948</c:v>
+                  <c:v>17.517542033343197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2673,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AY22" sqref="AY22"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3:AR17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3001,22 +3003,22 @@
         <v>ATM_EQ_SW</v>
       </c>
       <c r="AM3" s="78">
-        <v>13.837845058209499</v>
+        <v>14.507296403776699</v>
       </c>
       <c r="AN3" s="78">
-        <v>-2.16465516902328</v>
+        <v>-2.8341104356237601</v>
       </c>
       <c r="AO3" s="78">
-        <v>16.002500227232701</v>
+        <v>17.341406839400399</v>
       </c>
       <c r="AP3" s="78">
-        <v>5.8365949445930898</v>
+        <v>5.8365929840764599</v>
       </c>
       <c r="AQ3" s="78">
-        <v>24.2603773951218</v>
+        <v>24.260415341105201</v>
       </c>
       <c r="AR3" s="78">
-        <v>47.550916076763798</v>
+        <v>47.550991287681498</v>
       </c>
       <c r="AS3" s="42" t="s">
         <v>100</v>
@@ -3024,27 +3026,27 @@
       <c r="AT3" s="69"/>
       <c r="AU3" s="78">
         <f>AM3*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>14.759734209486618</v>
+        <v>14.761625301636297</v>
       </c>
       <c r="AV3" s="78">
         <f>AN3*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-3.0610895295431009</v>
+        <v>-3.0632586454245847</v>
       </c>
       <c r="AW3" s="78">
         <f>AU3-AV3</f>
-        <v>17.82082373902972</v>
+        <v>17.824883947060883</v>
       </c>
       <c r="AX3" s="78">
         <f>AVERAGE(AU3:AV3)</f>
-        <v>5.8493223399717582</v>
+        <v>5.8491833281058563</v>
       </c>
       <c r="AY3" s="78">
         <f>AQ3*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>23.28974545578863</v>
+        <v>23.289764134703894</v>
       </c>
       <c r="AZ3" s="78">
         <f>AR3*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>45.62763132064314</v>
+        <v>45.627668217487106</v>
       </c>
       <c r="BA3" s="69"/>
       <c r="BB3" s="69"/>
@@ -3153,22 +3155,22 @@
         <v>S2_ref_1</v>
       </c>
       <c r="AM4" s="82">
-        <v>5.5054466069134902</v>
+        <v>6.1687098916998204</v>
       </c>
       <c r="AN4" s="82">
-        <v>-12.0924502848762</v>
+        <v>-12.755717850561499</v>
       </c>
       <c r="AO4" s="82">
-        <v>17.597896891789699</v>
+        <v>18.924427742261301</v>
       </c>
       <c r="AP4" s="82">
-        <v>-3.2935018389813799</v>
+        <v>-3.29350397943085</v>
       </c>
       <c r="AQ4" s="82">
-        <v>17.6812819742809</v>
+        <v>17.6813234028828</v>
       </c>
       <c r="AR4" s="82">
-        <v>34.550094218463101</v>
+        <v>34.550175837285003</v>
       </c>
       <c r="AS4" s="42" t="s">
         <v>119</v>
@@ -3176,27 +3178,27 @@
       <c r="AT4" s="69"/>
       <c r="AU4" s="78">
         <f>AM4*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>6.3161233799249326</v>
+        <v>6.3130793987045815</v>
       </c>
       <c r="AV4" s="78">
         <f>AN4*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-12.372403732904573</v>
+        <v>-12.371611409865192</v>
       </c>
       <c r="AW4" s="78">
         <f t="shared" ref="AW4:AW17" si="10">AU4-AV4</f>
-        <v>18.688527112829505</v>
+        <v>18.684690808569773</v>
       </c>
       <c r="AX4" s="78">
         <f t="shared" ref="AX4:AX17" si="11">AVERAGE(AU4:AV4)</f>
-        <v>-3.0281401764898201</v>
+        <v>-3.0292660055803053</v>
       </c>
       <c r="AY4" s="78">
         <f>AQ4*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>16.940962612526206</v>
+        <v>16.940969363932343</v>
       </c>
       <c r="AZ4" s="78">
         <f>AR4*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>33.092346043334764</v>
+        <v>33.092359428486049</v>
       </c>
       <c r="BA4" s="69"/>
       <c r="BB4" s="69"/>
@@ -3310,48 +3312,48 @@
         <v>B6_ref_1</v>
       </c>
       <c r="AM5" s="82">
-        <v>-1.5458648044796</v>
+        <v>-0.87881766165753805</v>
       </c>
       <c r="AN5" s="82">
-        <v>2.2271825789230899</v>
+        <v>1.56013616507433</v>
       </c>
       <c r="AO5" s="82">
-        <v>-3.7730473834026799</v>
+        <v>-2.4389538267318698</v>
       </c>
       <c r="AP5" s="82">
-        <v>0.34065888722174398</v>
+        <v>0.340659251708397</v>
       </c>
       <c r="AQ5" s="82">
-        <v>22.603672551350499</v>
+        <v>22.6036654966768</v>
       </c>
       <c r="AR5" s="82">
-        <v>44.269731766645201</v>
+        <v>44.269717805129403</v>
       </c>
       <c r="AS5" s="42"/>
       <c r="AT5" s="69"/>
       <c r="AU5" s="78">
         <f>AM5*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>-0.82930176313097159</v>
+        <v>-0.82738259092413968</v>
       </c>
       <c r="AV5" s="78">
         <f>AN5*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>1.0580306501241861</v>
+        <v>1.0593795302866329</v>
       </c>
       <c r="AW5" s="78">
         <f t="shared" si="10"/>
-        <v>-1.8873324132551577</v>
+        <v>-1.8867621212107726</v>
       </c>
       <c r="AX5" s="78">
         <f t="shared" si="11"/>
-        <v>0.11436444349660724</v>
+        <v>0.11599846968124661</v>
       </c>
       <c r="AY5" s="78">
         <f>AQ5*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>21.691036421235573</v>
+        <v>21.691007824934864</v>
       </c>
       <c r="AZ5" s="78">
         <f>AR5*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>42.463940453784289</v>
+        <v>42.46388387781348</v>
       </c>
       <c r="BA5" s="69"/>
       <c r="BB5" s="69"/>
@@ -3469,48 +3471,48 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="AM6" s="78">
-        <v>13.624539536088299</v>
+        <v>14.2946169156188</v>
       </c>
       <c r="AN6" s="78">
-        <v>-0.44284175578310597</v>
+        <v>-1.1129226043251601</v>
       </c>
       <c r="AO6" s="78">
-        <v>14.067381291871399</v>
+        <v>15.407539519944001</v>
       </c>
       <c r="AP6" s="78">
-        <v>6.5908488901525999</v>
+        <v>6.5908471556468404</v>
       </c>
       <c r="AQ6" s="78">
-        <v>24.352429878149199</v>
+        <v>24.352463449670601</v>
       </c>
       <c r="AR6" s="78">
-        <v>47.733376584516698</v>
+        <v>47.733443130631599</v>
       </c>
       <c r="AS6" s="42"/>
       <c r="AT6" s="69"/>
       <c r="AU6" s="78">
         <f>AM6*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>14.543581702244511</v>
+        <v>14.546141248588258</v>
       </c>
       <c r="AV6" s="78">
         <f>AN6*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-1.4461946306102322</v>
+        <v>-1.4484574506637058</v>
       </c>
       <c r="AW6" s="78">
         <f t="shared" si="10"/>
-        <v>15.989776332854744</v>
+        <v>15.994598699251963</v>
       </c>
       <c r="AX6" s="78">
         <f t="shared" si="11"/>
-        <v>6.5486935358171392</v>
+        <v>6.5488418989622765</v>
       </c>
       <c r="AY6" s="78">
         <f>AQ6*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>23.378575482949014</v>
+        <v>23.378590154435322</v>
       </c>
       <c r="AZ6" s="78">
         <f>AR6*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>45.803558238299111</v>
+        <v>45.80358719727942</v>
       </c>
       <c r="BA6" s="69"/>
       <c r="BB6" s="69"/>
@@ -3628,48 +3630,48 @@
         <v>S2_ref_2</v>
       </c>
       <c r="AM7" s="78">
-        <v>5.2915702148271899</v>
+        <v>5.9548084033678199</v>
       </c>
       <c r="AN7" s="78">
-        <v>-12.0104270284902</v>
+        <v>-12.6736694280125</v>
       </c>
       <c r="AO7" s="78">
-        <v>17.301997243317398</v>
+        <v>18.628477831380302</v>
       </c>
       <c r="AP7" s="78">
-        <v>-3.3594284068315101</v>
+        <v>-3.35943051232235</v>
       </c>
       <c r="AQ7" s="78">
-        <v>17.7806714278295</v>
+        <v>17.780712179800201</v>
       </c>
       <c r="AR7" s="78">
-        <v>34.745911145374301</v>
+        <v>34.745991438514203</v>
       </c>
       <c r="AS7" s="42"/>
       <c r="AT7" s="69"/>
       <c r="AU7" s="78">
         <f>AM7*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>6.0993923833261592</v>
+        <v>6.0963572311932186</v>
       </c>
       <c r="AV7" s="78">
         <f>AN7*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-12.29547383021416</v>
+        <v>-12.294634401109324</v>
       </c>
       <c r="AW7" s="78">
         <f t="shared" si="10"/>
-        <v>18.394866213540318</v>
+        <v>18.390991632302544</v>
       </c>
       <c r="AX7" s="78">
         <f t="shared" si="11"/>
-        <v>-3.0980407234440004</v>
+        <v>-3.0991385849580526</v>
       </c>
       <c r="AY7" s="78">
         <f>AQ7*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>17.036872766905748</v>
+        <v>17.036879096322714</v>
       </c>
       <c r="AZ7" s="78">
         <f>AR7*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>33.281151110253703</v>
+        <v>33.281163664380117</v>
       </c>
       <c r="BA7" s="69"/>
       <c r="BB7" s="69"/>
@@ -3778,48 +3780,48 @@
         <v>B6_ref_2</v>
       </c>
       <c r="AM8" s="83">
-        <v>-2.19025748922324</v>
+        <v>-1.52410042474005</v>
       </c>
       <c r="AN8" s="83">
-        <v>0.42265552747914598</v>
+        <v>-0.243501080290143</v>
       </c>
       <c r="AO8" s="83">
-        <v>-2.61291301670239</v>
+        <v>-1.28059934444991</v>
       </c>
       <c r="AP8" s="83">
-        <v>-0.88380098087204795</v>
+        <v>-0.88380075251509604</v>
       </c>
       <c r="AQ8" s="83">
-        <v>21.5940737361231</v>
+        <v>21.594069316251701</v>
       </c>
       <c r="AR8" s="83">
-        <v>42.272615580605901</v>
+        <v>42.272606841582601</v>
       </c>
       <c r="AS8" s="42"/>
       <c r="AT8" s="69"/>
       <c r="AU8" s="78">
         <f>AM8*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>-1.4822951459120652</v>
+        <v>-1.4811745778966856</v>
       </c>
       <c r="AV8" s="78">
         <f>AN8*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-0.63444166305131089</v>
+        <v>-0.63277487945744493</v>
       </c>
       <c r="AW8" s="78">
         <f t="shared" si="10"/>
-        <v>-0.84785348286075435</v>
+        <v>-0.84839969843924068</v>
       </c>
       <c r="AX8" s="78">
         <f t="shared" si="11"/>
-        <v>-1.0583684044816881</v>
+        <v>-1.0569747286770652</v>
       </c>
       <c r="AY8" s="78">
         <f>AQ8*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>20.716780353085323</v>
+        <v>20.716751953294676</v>
       </c>
       <c r="AZ8" s="78">
         <f>AR8*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>40.538337488311079</v>
+        <v>40.538281386994711</v>
       </c>
       <c r="BA8" s="69"/>
       <c r="BB8" s="69"/>
@@ -3927,47 +3929,47 @@
         <v>ATM_EQ_SW_2</v>
       </c>
       <c r="AM9" s="82">
-        <v>14.7204185921359</v>
+        <v>15.3893026798115</v>
       </c>
       <c r="AN9" s="82">
-        <v>-4.19292836172629</v>
+        <v>-4.8618170550132103</v>
       </c>
       <c r="AO9" s="82">
-        <v>18.913346953862199</v>
+        <v>20.251119734824702</v>
       </c>
       <c r="AP9" s="82">
-        <v>5.2637451152047898</v>
+        <v>5.2637428123991601</v>
       </c>
       <c r="AQ9" s="82">
-        <v>23.3079288441653</v>
+        <v>23.307973415184001</v>
       </c>
       <c r="AR9" s="82">
-        <v>45.6639367309728</v>
+        <v>45.664024995999597</v>
       </c>
       <c r="AS9" s="75"/>
       <c r="AU9" s="78">
         <f>AM9*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>15.654087437132182</v>
+        <v>15.655262430538363</v>
       </c>
       <c r="AV9" s="78">
         <f>AN9*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-4.9634141411132422</v>
+        <v>-4.9656326990130326</v>
       </c>
       <c r="AW9" s="78">
         <f t="shared" si="10"/>
-        <v>20.617501578245424</v>
+        <v>20.620895129551396</v>
       </c>
       <c r="AX9" s="78">
         <f t="shared" si="11"/>
-        <v>5.3453366480094697</v>
+        <v>5.3448148657626646</v>
       </c>
       <c r="AY9" s="78">
         <f>AQ9*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>22.370639008381321</v>
+        <v>22.370661867167275</v>
       </c>
       <c r="AZ9" s="78">
         <f>AR9*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>43.808221388741295</v>
+        <v>43.808266562958778</v>
       </c>
     </row>
     <row r="10" spans="1:54">
@@ -4073,47 +4075,47 @@
         <v>DI</v>
       </c>
       <c r="AM10" s="78">
-        <v>12.5296145068617</v>
+        <v>13.1869461661054</v>
       </c>
       <c r="AN10" s="78">
-        <v>-31.800722793578199</v>
+        <v>-32.458064853802199</v>
       </c>
       <c r="AO10" s="78">
-        <v>44.33033730044</v>
+        <v>45.645011019907599</v>
       </c>
       <c r="AP10" s="78">
-        <v>-9.6355541433582399</v>
+        <v>-9.63555934384841</v>
       </c>
       <c r="AQ10" s="78">
-        <v>23.011923180081201</v>
+        <v>23.0120238360545</v>
       </c>
       <c r="AR10" s="78">
-        <v>45.077829352134998</v>
+        <v>45.078028629425901</v>
       </c>
       <c r="AS10" s="75"/>
       <c r="AU10" s="78">
         <f>AM10*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>13.434042727557351</v>
+        <v>13.423863850728907</v>
       </c>
       <c r="AV10" s="78">
         <f>AN10*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-30.856862325423542</v>
+        <v>-30.856156153841496</v>
       </c>
       <c r="AW10" s="78">
         <f t="shared" si="10"/>
-        <v>44.290905052980889</v>
+        <v>44.280020004570403</v>
       </c>
       <c r="AX10" s="78">
         <f t="shared" si="11"/>
-        <v>-8.7114097989330954</v>
+        <v>-8.7161461515562948</v>
       </c>
       <c r="AY10" s="78">
         <f>AQ10*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>22.084995532882765</v>
+        <v>22.085071825557812</v>
       </c>
       <c r="AZ10" s="78">
         <f>AR10*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>43.243101485019487</v>
+        <v>43.243252358099042</v>
       </c>
     </row>
     <row r="11" spans="1:54">
@@ -4219,47 +4221,47 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="AM11" s="82">
-        <v>15.8309907320658</v>
+        <v>16.5002615069154</v>
       </c>
       <c r="AN11" s="82">
-        <v>-3.9731856475206002</v>
+        <v>-4.6424612409758899</v>
       </c>
       <c r="AO11" s="82">
-        <v>19.804176379586401</v>
+        <v>21.142722747891298</v>
       </c>
       <c r="AP11" s="82">
-        <v>5.9289025422726001</v>
+        <v>5.9289001329697602</v>
       </c>
       <c r="AQ11" s="82">
-        <v>23.171307203657499</v>
+        <v>23.1713538359399</v>
       </c>
       <c r="AR11" s="82">
-        <v>45.393398658799804</v>
+        <v>45.393490994230802</v>
       </c>
       <c r="AS11" s="69"/>
       <c r="AU11" s="78">
         <f>AM11*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>16.779482364239044</v>
+        <v>16.780871265256408</v>
       </c>
       <c r="AV11" s="78">
         <f>AN11*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-4.7573166711320791</v>
+        <v>-4.7598352699677893</v>
       </c>
       <c r="AW11" s="78">
         <f t="shared" si="10"/>
-        <v>21.536799035371125</v>
+        <v>21.540706535224196</v>
       </c>
       <c r="AX11" s="78">
         <f t="shared" si="11"/>
-        <v>6.0110828465534825</v>
+        <v>6.0105179976443095</v>
       </c>
       <c r="AY11" s="78">
         <f>AQ11*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>22.238800043935441</v>
+        <v>22.238824574356268</v>
       </c>
       <c r="AZ11" s="78">
         <f>AR11*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>43.547370809445319</v>
+        <v>43.547419290490758</v>
       </c>
     </row>
     <row r="12" spans="1:54">
@@ -4365,47 +4367,47 @@
         <v>S2_ref_1</v>
       </c>
       <c r="AM12" s="82">
-        <v>5.6303612459263199</v>
+        <v>6.2934023168454996</v>
       </c>
       <c r="AN12" s="82">
-        <v>-12.7369578551756</v>
+        <v>-13.4000033884264</v>
       </c>
       <c r="AO12" s="82">
-        <v>18.367319101101899</v>
+        <v>19.6934057052719</v>
       </c>
       <c r="AP12" s="82">
-        <v>-3.55329830462462</v>
+        <v>-3.5533005357904499</v>
       </c>
       <c r="AQ12" s="82">
-        <v>17.047650523571001</v>
+        <v>17.047693707994899</v>
       </c>
       <c r="AR12" s="82">
-        <v>33.302136344730599</v>
+        <v>33.302221373024103</v>
       </c>
       <c r="AS12" s="69"/>
       <c r="AU12" s="78">
         <f>AM12*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>6.4427052524679418</v>
+        <v>6.4394161196902537</v>
       </c>
       <c r="AV12" s="78">
         <f>AN12*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-12.976889665931125</v>
+        <v>-12.976073652388976</v>
       </c>
       <c r="AW12" s="78">
         <f t="shared" si="10"/>
-        <v>19.419594918399067</v>
+        <v>19.41548977207923</v>
       </c>
       <c r="AX12" s="78">
         <f t="shared" si="11"/>
-        <v>-3.2670922067315917</v>
+        <v>-3.2683287663493612</v>
       </c>
       <c r="AY12" s="78">
         <f>AQ12*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>16.329512523130131</v>
+        <v>16.329519496491091</v>
       </c>
       <c r="AZ12" s="78">
         <f>AR12*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>31.889075347697002</v>
+        <v>31.889089170261926</v>
       </c>
     </row>
     <row r="13" spans="1:54">
@@ -4511,47 +4513,47 @@
         <v>B6_ref_1</v>
       </c>
       <c r="AM13" s="82">
-        <v>-0.95197073077611605</v>
+        <v>-0.28516347773321898</v>
       </c>
       <c r="AN13" s="82">
-        <v>1.2195527286622301</v>
+        <v>0.552745828694023</v>
       </c>
       <c r="AO13" s="82">
-        <v>-2.1715234594383501</v>
+        <v>-0.83790930642724304</v>
       </c>
       <c r="AP13" s="82">
-        <v>0.13379099894305799</v>
+        <v>0.13379117548040201</v>
       </c>
       <c r="AQ13" s="82">
-        <v>22.459159738802899</v>
+        <v>22.459156321907901</v>
       </c>
       <c r="AR13" s="82">
-        <v>43.983753381824997</v>
+        <v>43.983746620533097</v>
       </c>
       <c r="AS13" s="69"/>
       <c r="AU13" s="78">
         <f>AM13*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>-0.22748099547969858</v>
+        <v>-0.22589999958949991</v>
       </c>
       <c r="AV13" s="78">
         <f>AN13*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>0.11297104454439499</v>
+        <v>0.11425600036361094</v>
       </c>
       <c r="AW13" s="78">
         <f t="shared" si="10"/>
-        <v>-0.34045204002409357</v>
+        <v>-0.34015599995311085</v>
       </c>
       <c r="AX13" s="78">
         <f t="shared" si="11"/>
-        <v>-5.7254975467651792E-2</v>
+        <v>-5.5821999612944484E-2</v>
       </c>
       <c r="AY13" s="78">
         <f>AQ13*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>21.551582528831542</v>
+        <v>21.551557107158576</v>
       </c>
       <c r="AZ13" s="78">
         <f>AR13*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>42.188202452299684</v>
+        <v>42.188152165649086</v>
       </c>
     </row>
     <row r="14" spans="1:54">
@@ -4657,46 +4659,46 @@
         <v>ATM_EQ_SW_2</v>
       </c>
       <c r="AM14" s="84">
-        <v>13.1212595032093</v>
+        <v>13.790176235485999</v>
       </c>
       <c r="AN14" s="84">
-        <v>-3.0245950750757999</v>
+        <v>-3.6935157629354198</v>
       </c>
       <c r="AO14" s="84">
-        <v>16.1458545782851</v>
+        <v>17.483691998421399</v>
       </c>
       <c r="AP14" s="84">
-        <v>5.0483322140667397</v>
+        <v>5.0483302362752696</v>
       </c>
       <c r="AQ14" s="84">
-        <v>23.1234883652725</v>
+        <v>23.123526645611602</v>
       </c>
       <c r="AR14" s="84">
-        <v>45.298715835012402</v>
+        <v>45.298791629643702</v>
       </c>
       <c r="AU14" s="78">
         <f>AM14*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>14.033584399456103</v>
+        <v>14.035048602941941</v>
       </c>
       <c r="AV14" s="78">
         <f>AN14*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-3.8676302133328111</v>
+        <v>-3.869544121124056</v>
       </c>
       <c r="AW14" s="78">
         <f t="shared" si="10"/>
-        <v>17.901214612788912</v>
+        <v>17.904592724065999</v>
       </c>
       <c r="AX14" s="78">
         <f t="shared" si="11"/>
-        <v>5.082977093061646</v>
+        <v>5.0827522409089427</v>
       </c>
       <c r="AY14" s="78">
         <f>AQ14*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>22.192655186427871</v>
+        <v>22.19267154614079</v>
       </c>
       <c r="AZ14" s="78">
         <f>AR14*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>43.456078411166786</v>
+        <v>43.456110727443253</v>
       </c>
     </row>
     <row r="15" spans="1:54">
@@ -4802,46 +4804,46 @@
         <v>ATM_EQ_SW_3</v>
       </c>
       <c r="AM15" s="83">
-        <v>15.3661695705781</v>
+        <v>16.0354104426772</v>
       </c>
       <c r="AN15" s="83">
-        <v>-3.7328175302236501</v>
+        <v>-4.4020630524725899</v>
       </c>
       <c r="AO15" s="83">
-        <v>19.0989871008017</v>
+        <v>20.437473495149799</v>
       </c>
       <c r="AP15" s="83">
-        <v>5.8166760201772103</v>
+        <v>5.8166736951022999</v>
       </c>
       <c r="AQ15" s="83">
-        <v>23.703556787671602</v>
+        <v>23.703601789713598</v>
       </c>
       <c r="AR15" s="83">
-        <v>46.447550009369102</v>
+        <v>46.4476391602795</v>
       </c>
       <c r="AU15" s="78">
         <f>AM15*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>16.308457242734377</v>
+        <v>16.309890296412938</v>
       </c>
       <c r="AV15" s="78">
         <f>AN15*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-4.5318745625365429</v>
+        <v>-4.534296095826293</v>
       </c>
       <c r="AW15" s="78">
         <f t="shared" si="10"/>
-        <v>20.840331805270921</v>
+        <v>20.84418639223923</v>
       </c>
       <c r="AX15" s="78">
         <f t="shared" si="11"/>
-        <v>5.8882913400989167</v>
+        <v>5.8877971002933229</v>
       </c>
       <c r="AY15" s="78">
         <f>AQ15*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>22.752417313661923</v>
+        <v>22.752441507726758</v>
       </c>
       <c r="AZ15" s="78">
         <f>AR15*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>44.563774852887327</v>
+        <v>44.563822670816919</v>
       </c>
     </row>
     <row r="16" spans="1:54">
@@ -4947,46 +4949,46 @@
         <v>S2_ref_2</v>
       </c>
       <c r="AM16" s="83">
-        <v>5.7119699629923302</v>
+        <v>6.3749139427560202</v>
       </c>
       <c r="AN16" s="83">
-        <v>-13.036924129201299</v>
+        <v>-13.699872657930801</v>
       </c>
       <c r="AO16" s="83">
-        <v>18.748894092193702</v>
+        <v>20.074786600686799</v>
       </c>
       <c r="AP16" s="83">
-        <v>-3.6624770831045002</v>
+        <v>-3.6624793575874</v>
       </c>
       <c r="AQ16" s="83">
-        <v>17.560394819866399</v>
+        <v>17.5604388426949</v>
       </c>
       <c r="AR16" s="83">
-        <v>34.311946735499298</v>
+        <v>34.312033455564404</v>
       </c>
       <c r="AU16" s="78">
         <f>AM16*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>6.5254031996716098</v>
+        <v>6.522002624265129</v>
       </c>
       <c r="AV16" s="78">
         <f>AN16*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-13.258229096818942</v>
+        <v>-13.257407999438382</v>
       </c>
       <c r="AW16" s="78">
         <f t="shared" si="10"/>
-        <v>19.783632296490552</v>
+        <v>19.779410623703512</v>
       </c>
       <c r="AX16" s="78">
         <f t="shared" si="11"/>
-        <v>-3.3664129485736662</v>
+        <v>-3.3677026875866263</v>
       </c>
       <c r="AY16" s="78">
         <f>AQ16*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>16.824307321361651</v>
+        <v>16.824316295272638</v>
       </c>
       <c r="AZ16" s="78">
         <f>AR16*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>32.862726203176869</v>
+        <v>32.862743963055777</v>
       </c>
     </row>
     <row r="17" spans="1:52">
@@ -5092,46 +5094,46 @@
         <v>DI</v>
       </c>
       <c r="AM17" s="84">
-        <v>11.943231846484601</v>
+        <v>12.602797642375901</v>
       </c>
       <c r="AN17" s="84">
-        <v>-25.7762967852962</v>
+        <v>-26.435871486921201</v>
       </c>
       <c r="AO17" s="84">
-        <v>37.719528631780797</v>
+        <v>39.038669129297098</v>
       </c>
       <c r="AP17" s="84">
-        <v>-6.9165324694058299</v>
+        <v>-6.9165369222726198</v>
       </c>
       <c r="AQ17" s="84">
-        <v>22.706668195684699</v>
+        <v>22.706754381338399</v>
       </c>
       <c r="AR17" s="84">
-        <v>44.473574396293898</v>
+        <v>44.473744977690203</v>
       </c>
       <c r="AU17" s="78">
         <f>AM17*scale_decompression!B$14+scale_decompression!B$15</f>
-        <v>12.839833627936441</v>
+        <v>12.832012268963728</v>
       </c>
       <c r="AV17" s="78">
         <f>AN17*scale_decompression!C$14+scale_decompression!C$15</f>
-        <v>-25.206531833767624</v>
+        <v>-25.206194617346412</v>
       </c>
       <c r="AW17" s="78">
         <f t="shared" si="10"/>
-        <v>38.046365461704063</v>
+        <v>38.038206886310142</v>
       </c>
       <c r="AX17" s="78">
         <f t="shared" si="11"/>
-        <v>-6.1833491029155914</v>
+        <v>-6.1870911741913419</v>
       </c>
       <c r="AY17" s="78">
         <f>AQ17*scale_decompression!F$14+scale_decompression!F$15</f>
-        <v>21.790426525475187</v>
+        <v>21.790488145017012</v>
       </c>
       <c r="AZ17" s="78">
         <f>AR17*scale_decompression!G$14+scale_decompression!G$15</f>
-        <v>42.660483837131366</v>
+        <v>42.660605661854987</v>
       </c>
     </row>
     <row r="18" spans="1:52">
@@ -6552,8 +6554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514E26BA-DB14-A849-83E2-BEF03A6D7889}">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6731,11 +6733,11 @@
         <v>7.8916056437981025E-2</v>
       </c>
       <c r="U4" s="9"/>
-      <c r="V4" s="61">
+      <c r="V4" s="93">
         <f>AVERAGE(P4:P27)</f>
         <v>0.17122614458781849</v>
       </c>
-      <c r="W4" s="62">
+      <c r="W4" s="94">
         <f>AVERAGE(Q4:Q27)</f>
         <v>7.8744793494495618E-2</v>
       </c>
@@ -7833,8 +7835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7985,27 +7987,27 @@
       </c>
       <c r="B9" s="85">
         <f>AVERAGE(size_correction!AM3,size_correction!AM6,size_correction!AM9,size_correction!AM11,size_correction!AM14,size_correction!AM15)</f>
-        <v>14.416870498714482</v>
+        <v>15.0861773640476</v>
       </c>
       <c r="C9" s="85">
         <f>AVERAGE(size_correction!AN3,size_correction!AN6,size_correction!AN9,size_correction!AN11,size_correction!AN14,size_correction!AN15)</f>
-        <v>-2.9218372565587871</v>
+        <v>-3.5911483585576711</v>
       </c>
       <c r="D9" s="85">
         <f>B9-C9</f>
-        <v>17.338707755273269</v>
+        <v>18.677325722605271</v>
       </c>
       <c r="E9" s="85">
         <f>(B9+C9)/2</f>
-        <v>5.7475166210778479</v>
+        <v>5.7475145027449646</v>
       </c>
       <c r="F9" s="85">
         <f>AVERAGE(size_correction!AQ3,size_correction!AQ6,size_correction!AQ9,size_correction!AQ11,size_correction!AQ14,size_correction!AQ15)</f>
-        <v>23.653181412339649</v>
+        <v>23.653222412870818</v>
       </c>
       <c r="G9" s="85">
         <f>AVERAGE(size_correction!AR3,size_correction!AR6,size_correction!AR9,size_correction!AR11,size_correction!AR14,size_correction!AR15)</f>
-        <v>46.347982315905767</v>
+        <v>46.348063533077784</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -8014,27 +8016,27 @@
       </c>
       <c r="B10" s="85">
         <f>AVERAGE(size_correction!AM5,size_correction!AM8,size_correction!AM13)</f>
-        <v>-1.5626976748263186</v>
+        <v>-0.89602718804360248</v>
       </c>
       <c r="C10" s="85">
         <f>AVERAGE(size_correction!AN5,size_correction!AN8,size_correction!AN13)</f>
-        <v>1.2897969450214886</v>
+        <v>0.6231269711594033</v>
       </c>
       <c r="D10" s="85">
         <f>B10-C10</f>
-        <v>-2.8524946198478069</v>
+        <v>-1.5191541592030058</v>
       </c>
       <c r="E10" s="85">
         <f>(B10+C10)/2</f>
-        <v>-0.13645036490241502</v>
+        <v>-0.13645010844209959</v>
       </c>
       <c r="F10" s="85">
         <f>AVERAGE(size_correction!AQ5,size_correction!AQ8,size_correction!AQ13)</f>
-        <v>22.218968675425501</v>
+        <v>22.218963711612133</v>
       </c>
       <c r="G10" s="85">
         <f>AVERAGE(size_correction!AR5,size_correction!AR8,size_correction!AR13)</f>
-        <v>43.508700243025373</v>
+        <v>43.508690422415036</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -8043,27 +8045,27 @@
       </c>
       <c r="B11" s="85">
         <f>AVERAGE(size_correction!AM4,size_correction!AM7,size_correction!AM12,size_correction!AM16)</f>
-        <v>5.5348370076648328</v>
+        <v>6.1979586386672905</v>
       </c>
       <c r="C11" s="85">
         <f>AVERAGE(size_correction!AN4,size_correction!AN7,size_correction!AN12,size_correction!AN16)</f>
-        <v>-12.469189824435823</v>
+        <v>-13.132315831232798</v>
       </c>
       <c r="D11" s="85">
         <f>B11-C11</f>
-        <v>18.004026832100656</v>
+        <v>19.33027446990009</v>
       </c>
       <c r="E11" s="85">
         <f>(B11+C11)/2</f>
-        <v>-3.467176408385495</v>
+        <v>-3.4671785962827539</v>
       </c>
       <c r="F11" s="85">
         <f>AVERAGE(size_correction!AQ4,size_correction!AQ7,size_correction!AQ12,size_correction!AQ16)</f>
-        <v>17.517499686386948</v>
+        <v>17.517542033343197</v>
       </c>
       <c r="G11" s="85">
         <f>AVERAGE(size_correction!AR4,size_correction!AR7,size_correction!AR12,size_correction!AR16)</f>
-        <v>34.227522111016825</v>
+        <v>34.22760552609693</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -8091,21 +8093,21 @@
       </c>
       <c r="B14" s="59">
         <f>SLOPE(B4:B6,B9:B11)</f>
-        <v>1.0133469827344104</v>
+        <v>1.0131868141795473</v>
       </c>
       <c r="C14" s="59">
         <f>SLOPE(C4:C6,C9:C11)</f>
-        <v>0.9379035419952374</v>
+        <v>0.93818999030602346</v>
       </c>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
       <c r="F14" s="59">
         <f>SLOPE(F4:F6,F9:F11)</f>
-        <v>0.96499327599826168</v>
+        <v>0.96499559975550753</v>
       </c>
       <c r="G14" s="59">
         <f t="shared" ref="G14" si="1">SLOPE(G4:G6,G9:G11)</f>
-        <v>0.96419175756222808</v>
+        <v>0.96419404127598496</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -8114,21 +8116,21 @@
       </c>
       <c r="B15" s="57">
         <f>INTERCEPT(B4:B6,B9:B11)</f>
-        <v>0.73719567220375026</v>
+        <v>6.3023875935380502E-2</v>
       </c>
       <c r="C15" s="57">
         <f>INTERCEPT(C4:C6,C9:C11)</f>
-        <v>-1.0308517793178673</v>
+        <v>-0.40432460330052944</v>
       </c>
       <c r="D15" s="57"/>
       <c r="E15" s="57"/>
       <c r="F15" s="57">
         <f>INTERCEPT(F4:F6,F9:F11)</f>
-        <v>-0.12135560368412968</v>
+        <v>-0.12142991770363665</v>
       </c>
       <c r="G15" s="57">
         <f t="shared" ref="G15" si="2">INTERCEPT(G4:G6,G9:G11)</f>
-        <v>-0.22057002510575074</v>
+        <v>-0.22071423886166741</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -8146,27 +8148,27 @@
       </c>
       <c r="B17" s="57">
         <f t="shared" ref="B17:C19" si="3">B$15+B$14*B9</f>
-        <v>15.346487892548804</v>
+        <v>15.348139857562369</v>
       </c>
       <c r="C17" s="57">
         <f t="shared" si="3"/>
-        <v>-3.771253291378001</v>
+        <v>-3.773504047003243</v>
       </c>
       <c r="D17" s="57">
         <f>B17-C17</f>
-        <v>19.117741183926807</v>
+        <v>19.121643904565612</v>
       </c>
       <c r="E17" s="57">
         <f>AVERAGE(B17:C17)</f>
-        <v>5.7876173005854019</v>
+        <v>5.7873179052795631</v>
       </c>
       <c r="F17" s="57">
         <f>F$15+F$14*F9</f>
-        <v>22.703805415190697</v>
+        <v>22.703825630755052</v>
       </c>
       <c r="G17" s="57">
         <f>G$15+G$14*G9</f>
-        <v>44.467772503530497</v>
+        <v>44.467812444412708</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -8175,27 +8177,27 @@
       </c>
       <c r="B18" s="57">
         <f t="shared" si="3"/>
-        <v>-0.84635930150757854</v>
+        <v>-0.84481905613677521</v>
       </c>
       <c r="C18" s="57">
         <f t="shared" si="3"/>
-        <v>0.17885334387242335</v>
+        <v>0.18028688373093293</v>
       </c>
       <c r="D18" s="57">
         <f>B18-C18</f>
-        <v>-1.0252126453800019</v>
+        <v>-1.025105939867708</v>
       </c>
       <c r="E18" s="57">
         <f t="shared" ref="E18:E19" si="4">AVERAGE(B18:C18)</f>
-        <v>-0.33375297881757759</v>
+        <v>-0.33226608620292114</v>
       </c>
       <c r="F18" s="57">
         <f t="shared" ref="F18:F19" si="5">F$15+F$14*F10</f>
-        <v>21.31979976771748</v>
+        <v>21.319772295129372</v>
       </c>
       <c r="G18" s="57">
         <f>G$15+G$14*G10</f>
-        <v>41.730160131465027</v>
+        <v>41.73010581015243</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -8204,27 +8206,27 @@
       </c>
       <c r="B19" s="57">
         <f t="shared" si="3"/>
-        <v>6.3459060538476608</v>
+        <v>6.3427138434632964</v>
       </c>
       <c r="C19" s="57">
         <f t="shared" si="3"/>
-        <v>-12.725749081467198</v>
+        <v>-12.724931865700466</v>
       </c>
       <c r="D19" s="57">
         <f>B19-C19</f>
-        <v>19.07165513531486</v>
+        <v>19.067645709163763</v>
       </c>
       <c r="E19" s="57">
         <f t="shared" si="4"/>
-        <v>-3.1899215138097685</v>
+        <v>-3.1911090111185847</v>
       </c>
       <c r="F19" s="57">
         <f t="shared" si="5"/>
-        <v>16.782913805980932</v>
+        <v>16.782921063004697</v>
       </c>
       <c r="G19" s="57">
         <f>G$15+G$14*G11</f>
-        <v>32.781324676115581</v>
+        <v>32.781339056545967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>